<commit_message>
Matrice du libéria modifié et matrice du Sénégal ajoutée
</commit_message>
<xml_diff>
--- a/Matrice intermédiare_ch2021/Matrice_intermediaire_Libéria.xlsx
+++ b/Matrice intermédiare_ch2021/Matrice_intermediaire_Libéria.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DELL\Documents\CH 2021\Libéria\Arranger\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DELL\Documents\CH 2021\Libéria\Dossier finale avec Mody\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90BBCE19-C465-4003-90F3-74DA9235CF13}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB3925D0-8B32-45A7-9818-76EA77B1348F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{903597CF-C564-4494-BE48-227A7BB8E62E}"/>
   </bookViews>
@@ -1356,7 +1356,7 @@
   <dimension ref="A1:CU17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="AT3" sqref="AT3"/>
+      <selection activeCell="AI4" sqref="AI4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1366,6 +1366,7 @@
     <col min="18" max="18" width="14.85546875" bestFit="1" customWidth="1"/>
     <col min="19" max="23" width="13.28515625" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="19.7109375" bestFit="1" customWidth="1"/>
     <col min="40" max="40" width="27.42578125" bestFit="1" customWidth="1"/>
     <col min="41" max="41" width="21" bestFit="1" customWidth="1"/>
     <col min="42" max="42" width="24.5703125" bestFit="1" customWidth="1"/>
@@ -1741,6 +1742,21 @@
       <c r="X2">
         <v>3</v>
       </c>
+      <c r="AE2">
+        <v>73.430000000000007</v>
+      </c>
+      <c r="AF2">
+        <v>7.38</v>
+      </c>
+      <c r="AG2">
+        <v>3.69</v>
+      </c>
+      <c r="AH2">
+        <v>15.5</v>
+      </c>
+      <c r="AI2">
+        <v>2</v>
+      </c>
       <c r="AJ2">
         <v>49.1</v>
       </c>
@@ -1868,6 +1884,21 @@
       <c r="X3">
         <v>3</v>
       </c>
+      <c r="AE3">
+        <v>46.74</v>
+      </c>
+      <c r="AF3">
+        <v>14.94</v>
+      </c>
+      <c r="AG3">
+        <v>31.03</v>
+      </c>
+      <c r="AH3">
+        <v>7.28</v>
+      </c>
+      <c r="AI3">
+        <v>3</v>
+      </c>
       <c r="AJ3">
         <v>23.4</v>
       </c>
@@ -1995,6 +2026,21 @@
       <c r="X4">
         <v>2</v>
       </c>
+      <c r="AE4">
+        <v>75</v>
+      </c>
+      <c r="AF4">
+        <v>6.45</v>
+      </c>
+      <c r="AG4">
+        <v>3.23</v>
+      </c>
+      <c r="AH4">
+        <v>15.32</v>
+      </c>
+      <c r="AI4">
+        <v>2</v>
+      </c>
       <c r="AJ4">
         <v>63.7</v>
       </c>
@@ -2124,6 +2170,21 @@
       <c r="X5">
         <v>3</v>
       </c>
+      <c r="AE5">
+        <v>47.58</v>
+      </c>
+      <c r="AF5">
+        <v>13.31</v>
+      </c>
+      <c r="AG5">
+        <v>22.18</v>
+      </c>
+      <c r="AH5">
+        <v>16.940000000000001</v>
+      </c>
+      <c r="AI5">
+        <v>3</v>
+      </c>
       <c r="AJ5">
         <v>50</v>
       </c>
@@ -2251,6 +2312,21 @@
       <c r="X6">
         <v>3</v>
       </c>
+      <c r="AE6">
+        <v>71.92</v>
+      </c>
+      <c r="AF6">
+        <v>12.69</v>
+      </c>
+      <c r="AG6">
+        <v>6.15</v>
+      </c>
+      <c r="AH6">
+        <v>9.23</v>
+      </c>
+      <c r="AI6">
+        <v>2</v>
+      </c>
       <c r="AJ6">
         <v>46.9</v>
       </c>
@@ -2378,6 +2454,21 @@
       <c r="X7">
         <v>4</v>
       </c>
+      <c r="AE7">
+        <v>61.69</v>
+      </c>
+      <c r="AF7">
+        <v>18.010000000000002</v>
+      </c>
+      <c r="AG7">
+        <v>12.64</v>
+      </c>
+      <c r="AH7">
+        <v>7.66</v>
+      </c>
+      <c r="AI7">
+        <v>3</v>
+      </c>
       <c r="AJ7">
         <v>33</v>
       </c>
@@ -2505,6 +2596,21 @@
       <c r="X8">
         <v>3</v>
       </c>
+      <c r="AE8">
+        <v>51.75</v>
+      </c>
+      <c r="AF8">
+        <v>8.56</v>
+      </c>
+      <c r="AG8">
+        <v>9.73</v>
+      </c>
+      <c r="AH8">
+        <v>29.96</v>
+      </c>
+      <c r="AI8">
+        <v>4</v>
+      </c>
       <c r="AJ8">
         <v>30</v>
       </c>
@@ -2632,6 +2738,21 @@
       <c r="X9">
         <v>3</v>
       </c>
+      <c r="AE9">
+        <v>58.96</v>
+      </c>
+      <c r="AF9">
+        <v>14.93</v>
+      </c>
+      <c r="AG9">
+        <v>20.149999999999999</v>
+      </c>
+      <c r="AH9">
+        <v>5.97</v>
+      </c>
+      <c r="AI9">
+        <v>3</v>
+      </c>
       <c r="AJ9">
         <v>30.6</v>
       </c>
@@ -2759,6 +2880,21 @@
       <c r="X10">
         <v>3</v>
       </c>
+      <c r="AE10">
+        <v>53.64</v>
+      </c>
+      <c r="AF10">
+        <v>24.52</v>
+      </c>
+      <c r="AG10">
+        <v>7.66</v>
+      </c>
+      <c r="AH10">
+        <v>14.18</v>
+      </c>
+      <c r="AI10">
+        <v>3</v>
+      </c>
       <c r="AJ10">
         <v>39.6</v>
       </c>
@@ -2884,6 +3020,21 @@
       <c r="X11">
         <v>4</v>
       </c>
+      <c r="AE11">
+        <v>59.62</v>
+      </c>
+      <c r="AF11">
+        <v>4.62</v>
+      </c>
+      <c r="AG11">
+        <v>13.85</v>
+      </c>
+      <c r="AH11">
+        <v>21.92</v>
+      </c>
+      <c r="AI11">
+        <v>4</v>
+      </c>
       <c r="AJ11">
         <v>33.5</v>
       </c>
@@ -3007,6 +3158,21 @@
         <v>2.2999999999999998</v>
       </c>
       <c r="X12">
+        <v>3</v>
+      </c>
+      <c r="AE12">
+        <v>45.56</v>
+      </c>
+      <c r="AF12">
+        <v>14.67</v>
+      </c>
+      <c r="AG12">
+        <v>30.5</v>
+      </c>
+      <c r="AH12">
+        <v>9.27</v>
+      </c>
+      <c r="AI12">
         <v>3</v>
       </c>
       <c r="AJ12">
@@ -3126,6 +3292,21 @@
       <c r="X13">
         <v>3</v>
       </c>
+      <c r="AE13">
+        <v>53.67</v>
+      </c>
+      <c r="AF13">
+        <v>25.87</v>
+      </c>
+      <c r="AG13">
+        <v>10.039999999999999</v>
+      </c>
+      <c r="AH13">
+        <v>10.42</v>
+      </c>
+      <c r="AI13">
+        <v>3</v>
+      </c>
       <c r="AJ13">
         <v>51.4</v>
       </c>
@@ -3243,6 +3424,21 @@
       <c r="X14">
         <v>4</v>
       </c>
+      <c r="AE14">
+        <v>45.77</v>
+      </c>
+      <c r="AF14">
+        <v>27.31</v>
+      </c>
+      <c r="AG14">
+        <v>11.15</v>
+      </c>
+      <c r="AH14">
+        <v>15.77</v>
+      </c>
+      <c r="AI14">
+        <v>3</v>
+      </c>
       <c r="AJ14">
         <v>27.7</v>
       </c>
@@ -3368,6 +3564,21 @@
       <c r="X15">
         <v>3</v>
       </c>
+      <c r="AE15">
+        <v>70</v>
+      </c>
+      <c r="AF15">
+        <v>9.23</v>
+      </c>
+      <c r="AG15">
+        <v>13.85</v>
+      </c>
+      <c r="AH15">
+        <v>6.92</v>
+      </c>
+      <c r="AI15">
+        <v>3</v>
+      </c>
       <c r="AJ15">
         <v>62.3</v>
       </c>
@@ -3493,6 +3704,21 @@
       <c r="X16">
         <v>4</v>
       </c>
+      <c r="AE16">
+        <v>54.23</v>
+      </c>
+      <c r="AF16">
+        <v>8.08</v>
+      </c>
+      <c r="AG16">
+        <v>21.92</v>
+      </c>
+      <c r="AH16">
+        <v>15.77</v>
+      </c>
+      <c r="AI16">
+        <v>3</v>
+      </c>
       <c r="AJ16">
         <v>28.5</v>
       </c>
@@ -3616,6 +3842,21 @@
         <v>2.2999999999999998</v>
       </c>
       <c r="X17">
+        <v>3</v>
+      </c>
+      <c r="AE17">
+        <v>50.38</v>
+      </c>
+      <c r="AF17">
+        <v>16.29</v>
+      </c>
+      <c r="AG17">
+        <v>18.940000000000001</v>
+      </c>
+      <c r="AH17">
+        <v>14.39</v>
+      </c>
+      <c r="AI17">
         <v>3</v>
       </c>
       <c r="AJ17">

</xml_diff>